<commit_message>
Tests the example1 code and it working fine
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,48 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aakf\Desktop\py\forproject\ProjectA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F041432B-3DCE-48C0-B6B2-0A92FA001A43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{69802644-5717-4E62-B2A3-38EABE7EA6E1}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -58,24 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -375,13 +351,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BE2E4F-5499-4E60-A170-52B980F29009}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="30"/>
+    <col customWidth="1" max="2" min="2" width="10"/>
+    <col customWidth="1" max="3" min="3" width="10"/>
+    <col customWidth="1" max="4" min="4" width="20"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
+    <col customWidth="1" max="6" min="6" width="40"/>
+    <col customWidth="1" max="7" min="7" width="50"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Course</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Form Number</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Contact Number</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Email id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Aaakef</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>kjkjl</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>kjkjk</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nnnnnn</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>mmmm</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>mm333</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>